<commit_message>
Minor fix in ws_6 chart
</commit_message>
<xml_diff>
--- a/logs/charts_results_files/data_ws_6.xlsx
+++ b/logs/charts_results_files/data_ws_6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joela\crc-p2\logs\charts_results_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49652386-984E-4402-BB35-C144CABDCEB2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636275CC-5A7E-44A2-8731-CA9CE3675E55}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6030" xr2:uid="{7BCBB6FA-6256-42E5-835E-38D250AD9F33}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="5">
   <si>
     <t>Average degree</t>
   </si>
@@ -2595,7 +2595,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>